<commit_message>
Aggiornamento automatico - 2025-11-20 19:30:46
</commit_message>
<xml_diff>
--- a/template_excel.xlsx
+++ b/template_excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Generatore_Strutture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Generatore_Strutture\sito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE96A53-F590-4D5C-9876-8E7F4386620B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C23234-2D1E-4216-A81F-985CEA933B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1584" yWindow="864" windowWidth="18864" windowHeight="10548" xr2:uid="{E23BAD12-4D9A-44D5-BA43-3099214ED9E2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E23BAD12-4D9A-44D5-BA43-3099214ED9E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -170,8 +170,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2A362362-EAA3-449C-8564-3A37DA7D434B}" name="Table3" displayName="Table3" ref="A1:L18" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:L18" xr:uid="{2A362362-EAA3-449C-8564-3A37DA7D434B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2A362362-EAA3-449C-8564-3A37DA7D434B}" name="Table3" displayName="Table3" ref="A1:L127" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:L127" xr:uid="{2A362362-EAA3-449C-8564-3A37DA7D434B}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{80BD74C1-B7E7-4DC1-86EE-40720B30BA26}" name="Tag Name"/>
     <tableColumn id="2" xr3:uid="{23C3EE45-1155-4EF4-9707-F15C380299C3}" name="Data type"/>
@@ -510,7 +510,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>